<commit_message>
contents moved: dialog/ -> /index.html
</commit_message>
<xml_diff>
--- a/px-files/blogs/articles.xlsx
+++ b/px-files/blogs/articles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomk79/mydoc_TomK/projs/pickles2/pickles2/pickles2/px-files/blogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomk79/mydoc_TomK/projs/github/tomk79/app-inside-head/px-files/blogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42672F80-D37A-E546-BDA6-EC09ACACB79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065CDFCD-375F-D94C-83BB-E30ADEF1E81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sitemap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.2.1</t>
   </si>
@@ -53,18 +53,6 @@
   </si>
   <si>
     <t>layout</t>
-  </si>
-  <si>
-    <t>2023年のトレンド予測：持続可能なライフスタイルがますます重要に</t>
-  </si>
-  <si>
-    <t>/articles/2022/08/18_welcome/</t>
-  </si>
-  <si>
-    <t>ようこそ！ 記念すべき最初の記事をお読みください。</t>
-  </si>
-  <si>
-    <t>2022-08-18</t>
   </si>
   <si>
     <t>EndOfData</t>
@@ -100,10 +88,6 @@
   </si>
   <si>
     <t>「Pickles 2」 ブログマップ</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>article</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -211,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -220,8 +204,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -526,13 +508,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:YG12"/>
+  <dimension ref="A1:YG11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
@@ -1208,7 +1190,7 @@
     </row>
     <row r="3" spans="1:657" ht="38">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:657">
@@ -1227,16 +1209,16 @@
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:657">
@@ -1256,695 +1238,672 @@
         <v>6</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:657">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    <row r="11" spans="1:657" ht="5" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:657" ht="5" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
-      <c r="AO12" s="2"/>
-      <c r="AP12" s="2"/>
-      <c r="AQ12" s="2"/>
-      <c r="AR12" s="2"/>
-      <c r="AS12" s="2"/>
-      <c r="AT12" s="2"/>
-      <c r="AU12" s="2"/>
-      <c r="AV12" s="2"/>
-      <c r="AW12" s="2"/>
-      <c r="AX12" s="2"/>
-      <c r="AY12" s="2"/>
-      <c r="AZ12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BB12" s="2"/>
-      <c r="BC12" s="2"/>
-      <c r="BD12" s="2"/>
-      <c r="BE12" s="2"/>
-      <c r="BF12" s="2"/>
-      <c r="BG12" s="2"/>
-      <c r="BH12" s="2"/>
-      <c r="BI12" s="2"/>
-      <c r="BJ12" s="2"/>
-      <c r="BK12" s="2"/>
-      <c r="BL12" s="2"/>
-      <c r="BM12" s="2"/>
-      <c r="BN12" s="2"/>
-      <c r="BO12" s="2"/>
-      <c r="BP12" s="2"/>
-      <c r="BQ12" s="2"/>
-      <c r="BR12" s="2"/>
-      <c r="BS12" s="2"/>
-      <c r="BT12" s="2"/>
-      <c r="BU12" s="2"/>
-      <c r="BV12" s="2"/>
-      <c r="BW12" s="2"/>
-      <c r="BX12" s="2"/>
-      <c r="BY12" s="2"/>
-      <c r="BZ12" s="2"/>
-      <c r="CA12" s="2"/>
-      <c r="CB12" s="2"/>
-      <c r="CC12" s="2"/>
-      <c r="CD12" s="2"/>
-      <c r="CE12" s="2"/>
-      <c r="CF12" s="2"/>
-      <c r="CG12" s="2"/>
-      <c r="CH12" s="2"/>
-      <c r="CI12" s="2"/>
-      <c r="CJ12" s="2"/>
-      <c r="CK12" s="2"/>
-      <c r="CL12" s="2"/>
-      <c r="CM12" s="2"/>
-      <c r="CN12" s="2"/>
-      <c r="CO12" s="2"/>
-      <c r="CP12" s="2"/>
-      <c r="CQ12" s="2"/>
-      <c r="CR12" s="2"/>
-      <c r="CS12" s="2"/>
-      <c r="CT12" s="2"/>
-      <c r="CU12" s="2"/>
-      <c r="CV12" s="2"/>
-      <c r="CW12" s="2"/>
-      <c r="CX12" s="2"/>
-      <c r="CY12" s="2"/>
-      <c r="CZ12" s="2"/>
-      <c r="DA12" s="2"/>
-      <c r="DB12" s="2"/>
-      <c r="DC12" s="2"/>
-      <c r="DD12" s="2"/>
-      <c r="DE12" s="2"/>
-      <c r="DF12" s="2"/>
-      <c r="DG12" s="2"/>
-      <c r="DH12" s="2"/>
-      <c r="DI12" s="2"/>
-      <c r="DJ12" s="2"/>
-      <c r="DK12" s="2"/>
-      <c r="DL12" s="2"/>
-      <c r="DM12" s="2"/>
-      <c r="DN12" s="2"/>
-      <c r="DO12" s="2"/>
-      <c r="DP12" s="2"/>
-      <c r="DQ12" s="2"/>
-      <c r="DR12" s="2"/>
-      <c r="DS12" s="2"/>
-      <c r="DT12" s="2"/>
-      <c r="DU12" s="2"/>
-      <c r="DV12" s="2"/>
-      <c r="DW12" s="2"/>
-      <c r="DX12" s="2"/>
-      <c r="DY12" s="2"/>
-      <c r="DZ12" s="2"/>
-      <c r="EA12" s="2"/>
-      <c r="EB12" s="2"/>
-      <c r="EC12" s="2"/>
-      <c r="ED12" s="2"/>
-      <c r="EE12" s="2"/>
-      <c r="EF12" s="2"/>
-      <c r="EG12" s="2"/>
-      <c r="EH12" s="2"/>
-      <c r="EI12" s="2"/>
-      <c r="EJ12" s="2"/>
-      <c r="EK12" s="2"/>
-      <c r="EL12" s="2"/>
-      <c r="EM12" s="2"/>
-      <c r="EN12" s="2"/>
-      <c r="EO12" s="2"/>
-      <c r="EP12" s="2"/>
-      <c r="EQ12" s="2"/>
-      <c r="ER12" s="2"/>
-      <c r="ES12" s="2"/>
-      <c r="ET12" s="2"/>
-      <c r="EU12" s="2"/>
-      <c r="EV12" s="2"/>
-      <c r="EW12" s="2"/>
-      <c r="EX12" s="2"/>
-      <c r="EY12" s="2"/>
-      <c r="EZ12" s="2"/>
-      <c r="FA12" s="2"/>
-      <c r="FB12" s="2"/>
-      <c r="FC12" s="2"/>
-      <c r="FD12" s="2"/>
-      <c r="FE12" s="2"/>
-      <c r="FF12" s="2"/>
-      <c r="FG12" s="2"/>
-      <c r="FH12" s="2"/>
-      <c r="FI12" s="2"/>
-      <c r="FJ12" s="2"/>
-      <c r="FK12" s="2"/>
-      <c r="FL12" s="2"/>
-      <c r="FM12" s="2"/>
-      <c r="FN12" s="2"/>
-      <c r="FO12" s="2"/>
-      <c r="FP12" s="2"/>
-      <c r="FQ12" s="2"/>
-      <c r="FR12" s="2"/>
-      <c r="FS12" s="2"/>
-      <c r="FT12" s="2"/>
-      <c r="FU12" s="2"/>
-      <c r="FV12" s="2"/>
-      <c r="FW12" s="2"/>
-      <c r="FX12" s="2"/>
-      <c r="FY12" s="2"/>
-      <c r="FZ12" s="2"/>
-      <c r="GA12" s="2"/>
-      <c r="GB12" s="2"/>
-      <c r="GC12" s="2"/>
-      <c r="GD12" s="2"/>
-      <c r="GE12" s="2"/>
-      <c r="GF12" s="2"/>
-      <c r="GG12" s="2"/>
-      <c r="GH12" s="2"/>
-      <c r="GI12" s="2"/>
-      <c r="GJ12" s="2"/>
-      <c r="GK12" s="2"/>
-      <c r="GL12" s="2"/>
-      <c r="GM12" s="2"/>
-      <c r="GN12" s="2"/>
-      <c r="GO12" s="2"/>
-      <c r="GP12" s="2"/>
-      <c r="GQ12" s="2"/>
-      <c r="GR12" s="2"/>
-      <c r="GS12" s="2"/>
-      <c r="GT12" s="2"/>
-      <c r="GU12" s="2"/>
-      <c r="GV12" s="2"/>
-      <c r="GW12" s="2"/>
-      <c r="GX12" s="2"/>
-      <c r="GY12" s="2"/>
-      <c r="GZ12" s="2"/>
-      <c r="HA12" s="2"/>
-      <c r="HB12" s="2"/>
-      <c r="HC12" s="2"/>
-      <c r="HD12" s="2"/>
-      <c r="HE12" s="2"/>
-      <c r="HF12" s="2"/>
-      <c r="HG12" s="2"/>
-      <c r="HH12" s="2"/>
-      <c r="HI12" s="2"/>
-      <c r="HJ12" s="2"/>
-      <c r="HK12" s="2"/>
-      <c r="HL12" s="2"/>
-      <c r="HM12" s="2"/>
-      <c r="HN12" s="2"/>
-      <c r="HO12" s="2"/>
-      <c r="HP12" s="2"/>
-      <c r="HQ12" s="2"/>
-      <c r="HR12" s="2"/>
-      <c r="HS12" s="2"/>
-      <c r="HT12" s="2"/>
-      <c r="HU12" s="2"/>
-      <c r="HV12" s="2"/>
-      <c r="HW12" s="2"/>
-      <c r="HX12" s="2"/>
-      <c r="HY12" s="2"/>
-      <c r="HZ12" s="2"/>
-      <c r="IA12" s="2"/>
-      <c r="IB12" s="2"/>
-      <c r="IC12" s="2"/>
-      <c r="ID12" s="2"/>
-      <c r="IE12" s="2"/>
-      <c r="IF12" s="2"/>
-      <c r="IG12" s="2"/>
-      <c r="IH12" s="2"/>
-      <c r="II12" s="2"/>
-      <c r="IJ12" s="2"/>
-      <c r="IK12" s="2"/>
-      <c r="IL12" s="2"/>
-      <c r="IM12" s="2"/>
-      <c r="IN12" s="2"/>
-      <c r="IO12" s="2"/>
-      <c r="IP12" s="2"/>
-      <c r="IQ12" s="2"/>
-      <c r="IR12" s="2"/>
-      <c r="IS12" s="2"/>
-      <c r="IT12" s="2"/>
-      <c r="IU12" s="2"/>
-      <c r="IV12" s="2"/>
-      <c r="IW12" s="2"/>
-      <c r="IX12" s="2"/>
-      <c r="IY12" s="2"/>
-      <c r="IZ12" s="2"/>
-      <c r="JA12" s="2"/>
-      <c r="JB12" s="2"/>
-      <c r="JC12" s="2"/>
-      <c r="JD12" s="2"/>
-      <c r="JE12" s="2"/>
-      <c r="JF12" s="2"/>
-      <c r="JG12" s="2"/>
-      <c r="JH12" s="2"/>
-      <c r="JI12" s="2"/>
-      <c r="JJ12" s="2"/>
-      <c r="JK12" s="2"/>
-      <c r="JL12" s="2"/>
-      <c r="JM12" s="2"/>
-      <c r="JN12" s="2"/>
-      <c r="JO12" s="2"/>
-      <c r="JP12" s="2"/>
-      <c r="JQ12" s="2"/>
-      <c r="JR12" s="2"/>
-      <c r="JS12" s="2"/>
-      <c r="JT12" s="2"/>
-      <c r="JU12" s="2"/>
-      <c r="JV12" s="2"/>
-      <c r="JW12" s="2"/>
-      <c r="JX12" s="2"/>
-      <c r="JY12" s="2"/>
-      <c r="JZ12" s="2"/>
-      <c r="KA12" s="2"/>
-      <c r="KB12" s="2"/>
-      <c r="KC12" s="2"/>
-      <c r="KD12" s="2"/>
-      <c r="KE12" s="2"/>
-      <c r="KF12" s="2"/>
-      <c r="KG12" s="2"/>
-      <c r="KH12" s="2"/>
-      <c r="KI12" s="2"/>
-      <c r="KJ12" s="2"/>
-      <c r="KK12" s="2"/>
-      <c r="KL12" s="2"/>
-      <c r="KM12" s="2"/>
-      <c r="KN12" s="2"/>
-      <c r="KO12" s="2"/>
-      <c r="KP12" s="2"/>
-      <c r="KQ12" s="2"/>
-      <c r="KR12" s="2"/>
-      <c r="KS12" s="2"/>
-      <c r="KT12" s="2"/>
-      <c r="KU12" s="2"/>
-      <c r="KV12" s="2"/>
-      <c r="KW12" s="2"/>
-      <c r="KX12" s="2"/>
-      <c r="KY12" s="2"/>
-      <c r="KZ12" s="2"/>
-      <c r="LA12" s="2"/>
-      <c r="LB12" s="2"/>
-      <c r="LC12" s="2"/>
-      <c r="LD12" s="2"/>
-      <c r="LE12" s="2"/>
-      <c r="LF12" s="2"/>
-      <c r="LG12" s="2"/>
-      <c r="LH12" s="2"/>
-      <c r="LI12" s="2"/>
-      <c r="LJ12" s="2"/>
-      <c r="LK12" s="2"/>
-      <c r="LL12" s="2"/>
-      <c r="LM12" s="2"/>
-      <c r="LN12" s="2"/>
-      <c r="LO12" s="2"/>
-      <c r="LP12" s="2"/>
-      <c r="LQ12" s="2"/>
-      <c r="LR12" s="2"/>
-      <c r="LS12" s="2"/>
-      <c r="LT12" s="2"/>
-      <c r="LU12" s="2"/>
-      <c r="LV12" s="2"/>
-      <c r="LW12" s="2"/>
-      <c r="LX12" s="2"/>
-      <c r="LY12" s="2"/>
-      <c r="LZ12" s="2"/>
-      <c r="MA12" s="2"/>
-      <c r="MB12" s="2"/>
-      <c r="MC12" s="2"/>
-      <c r="MD12" s="2"/>
-      <c r="ME12" s="2"/>
-      <c r="MF12" s="2"/>
-      <c r="MG12" s="2"/>
-      <c r="MH12" s="2"/>
-      <c r="MI12" s="2"/>
-      <c r="MJ12" s="2"/>
-      <c r="MK12" s="2"/>
-      <c r="ML12" s="2"/>
-      <c r="MM12" s="2"/>
-      <c r="MN12" s="2"/>
-      <c r="MO12" s="2"/>
-      <c r="MP12" s="2"/>
-      <c r="MQ12" s="2"/>
-      <c r="MR12" s="2"/>
-      <c r="MS12" s="2"/>
-      <c r="MT12" s="2"/>
-      <c r="MU12" s="2"/>
-      <c r="MV12" s="2"/>
-      <c r="MW12" s="2"/>
-      <c r="MX12" s="2"/>
-      <c r="MY12" s="2"/>
-      <c r="MZ12" s="2"/>
-      <c r="NA12" s="2"/>
-      <c r="NB12" s="2"/>
-      <c r="NC12" s="2"/>
-      <c r="ND12" s="2"/>
-      <c r="NE12" s="2"/>
-      <c r="NF12" s="2"/>
-      <c r="NG12" s="2"/>
-      <c r="NH12" s="2"/>
-      <c r="NI12" s="2"/>
-      <c r="NJ12" s="2"/>
-      <c r="NK12" s="2"/>
-      <c r="NL12" s="2"/>
-      <c r="NM12" s="2"/>
-      <c r="NN12" s="2"/>
-      <c r="NO12" s="2"/>
-      <c r="NP12" s="2"/>
-      <c r="NQ12" s="2"/>
-      <c r="NR12" s="2"/>
-      <c r="NS12" s="2"/>
-      <c r="NT12" s="2"/>
-      <c r="NU12" s="2"/>
-      <c r="NV12" s="2"/>
-      <c r="NW12" s="2"/>
-      <c r="NX12" s="2"/>
-      <c r="NY12" s="2"/>
-      <c r="NZ12" s="2"/>
-      <c r="OA12" s="2"/>
-      <c r="OB12" s="2"/>
-      <c r="OC12" s="2"/>
-      <c r="OD12" s="2"/>
-      <c r="OE12" s="2"/>
-      <c r="OF12" s="2"/>
-      <c r="OG12" s="2"/>
-      <c r="OH12" s="2"/>
-      <c r="OI12" s="2"/>
-      <c r="OJ12" s="2"/>
-      <c r="OK12" s="2"/>
-      <c r="OL12" s="2"/>
-      <c r="OM12" s="2"/>
-      <c r="ON12" s="2"/>
-      <c r="OO12" s="2"/>
-      <c r="OP12" s="2"/>
-      <c r="OQ12" s="2"/>
-      <c r="OR12" s="2"/>
-      <c r="OS12" s="2"/>
-      <c r="OT12" s="2"/>
-      <c r="OU12" s="2"/>
-      <c r="OV12" s="2"/>
-      <c r="OW12" s="2"/>
-      <c r="OX12" s="2"/>
-      <c r="OY12" s="2"/>
-      <c r="OZ12" s="2"/>
-      <c r="PA12" s="2"/>
-      <c r="PB12" s="2"/>
-      <c r="PC12" s="2"/>
-      <c r="PD12" s="2"/>
-      <c r="PE12" s="2"/>
-      <c r="PF12" s="2"/>
-      <c r="PG12" s="2"/>
-      <c r="PH12" s="2"/>
-      <c r="PI12" s="2"/>
-      <c r="PJ12" s="2"/>
-      <c r="PK12" s="2"/>
-      <c r="PL12" s="2"/>
-      <c r="PM12" s="2"/>
-      <c r="PN12" s="2"/>
-      <c r="PO12" s="2"/>
-      <c r="PP12" s="2"/>
-      <c r="PQ12" s="2"/>
-      <c r="PR12" s="2"/>
-      <c r="PS12" s="2"/>
-      <c r="PT12" s="2"/>
-      <c r="PU12" s="2"/>
-      <c r="PV12" s="2"/>
-      <c r="PW12" s="2"/>
-      <c r="PX12" s="2"/>
-      <c r="PY12" s="2"/>
-      <c r="PZ12" s="2"/>
-      <c r="QA12" s="2"/>
-      <c r="QB12" s="2"/>
-      <c r="QC12" s="2"/>
-      <c r="QD12" s="2"/>
-      <c r="QE12" s="2"/>
-      <c r="QF12" s="2"/>
-      <c r="QG12" s="2"/>
-      <c r="QH12" s="2"/>
-      <c r="QI12" s="2"/>
-      <c r="QJ12" s="2"/>
-      <c r="QK12" s="2"/>
-      <c r="QL12" s="2"/>
-      <c r="QM12" s="2"/>
-      <c r="QN12" s="2"/>
-      <c r="QO12" s="2"/>
-      <c r="QP12" s="2"/>
-      <c r="QQ12" s="2"/>
-      <c r="QR12" s="2"/>
-      <c r="QS12" s="2"/>
-      <c r="QT12" s="2"/>
-      <c r="QU12" s="2"/>
-      <c r="QV12" s="2"/>
-      <c r="QW12" s="2"/>
-      <c r="QX12" s="2"/>
-      <c r="QY12" s="2"/>
-      <c r="QZ12" s="2"/>
-      <c r="RA12" s="2"/>
-      <c r="RB12" s="2"/>
-      <c r="RC12" s="2"/>
-      <c r="RD12" s="2"/>
-      <c r="RE12" s="2"/>
-      <c r="RF12" s="2"/>
-      <c r="RG12" s="2"/>
-      <c r="RH12" s="2"/>
-      <c r="RI12" s="2"/>
-      <c r="RJ12" s="2"/>
-      <c r="RK12" s="2"/>
-      <c r="RL12" s="2"/>
-      <c r="RM12" s="2"/>
-      <c r="RN12" s="2"/>
-      <c r="RO12" s="2"/>
-      <c r="RP12" s="2"/>
-      <c r="RQ12" s="2"/>
-      <c r="RR12" s="2"/>
-      <c r="RS12" s="2"/>
-      <c r="RT12" s="2"/>
-      <c r="RU12" s="2"/>
-      <c r="RV12" s="2"/>
-      <c r="RW12" s="2"/>
-      <c r="RX12" s="2"/>
-      <c r="RY12" s="2"/>
-      <c r="RZ12" s="2"/>
-      <c r="SA12" s="2"/>
-      <c r="SB12" s="2"/>
-      <c r="SC12" s="2"/>
-      <c r="SD12" s="2"/>
-      <c r="SE12" s="2"/>
-      <c r="SF12" s="2"/>
-      <c r="SG12" s="2"/>
-      <c r="SH12" s="2"/>
-      <c r="SI12" s="2"/>
-      <c r="SJ12" s="2"/>
-      <c r="SK12" s="2"/>
-      <c r="SL12" s="2"/>
-      <c r="SM12" s="2"/>
-      <c r="SN12" s="2"/>
-      <c r="SO12" s="2"/>
-      <c r="SP12" s="2"/>
-      <c r="SQ12" s="2"/>
-      <c r="SR12" s="2"/>
-      <c r="SS12" s="2"/>
-      <c r="ST12" s="2"/>
-      <c r="SU12" s="2"/>
-      <c r="SV12" s="2"/>
-      <c r="SW12" s="2"/>
-      <c r="SX12" s="2"/>
-      <c r="SY12" s="2"/>
-      <c r="SZ12" s="2"/>
-      <c r="TA12" s="2"/>
-      <c r="TB12" s="2"/>
-      <c r="TC12" s="2"/>
-      <c r="TD12" s="2"/>
-      <c r="TE12" s="2"/>
-      <c r="TF12" s="2"/>
-      <c r="TG12" s="2"/>
-      <c r="TH12" s="2"/>
-      <c r="TI12" s="2"/>
-      <c r="TJ12" s="2"/>
-      <c r="TK12" s="2"/>
-      <c r="TL12" s="2"/>
-      <c r="TM12" s="2"/>
-      <c r="TN12" s="2"/>
-      <c r="TO12" s="2"/>
-      <c r="TP12" s="2"/>
-      <c r="TQ12" s="2"/>
-      <c r="TR12" s="2"/>
-      <c r="TS12" s="2"/>
-      <c r="TT12" s="2"/>
-      <c r="TU12" s="2"/>
-      <c r="TV12" s="2"/>
-      <c r="TW12" s="2"/>
-      <c r="TX12" s="2"/>
-      <c r="TY12" s="2"/>
-      <c r="TZ12" s="2"/>
-      <c r="UA12" s="2"/>
-      <c r="UB12" s="2"/>
-      <c r="UC12" s="2"/>
-      <c r="UD12" s="2"/>
-      <c r="UE12" s="2"/>
-      <c r="UF12" s="2"/>
-      <c r="UG12" s="2"/>
-      <c r="UH12" s="2"/>
-      <c r="UI12" s="2"/>
-      <c r="UJ12" s="2"/>
-      <c r="UK12" s="2"/>
-      <c r="UL12" s="2"/>
-      <c r="UM12" s="2"/>
-      <c r="UN12" s="2"/>
-      <c r="UO12" s="2"/>
-      <c r="UP12" s="2"/>
-      <c r="UQ12" s="2"/>
-      <c r="UR12" s="2"/>
-      <c r="US12" s="2"/>
-      <c r="UT12" s="2"/>
-      <c r="UU12" s="2"/>
-      <c r="UV12" s="2"/>
-      <c r="UW12" s="2"/>
-      <c r="UX12" s="2"/>
-      <c r="UY12" s="2"/>
-      <c r="UZ12" s="2"/>
-      <c r="VA12" s="2"/>
-      <c r="VB12" s="2"/>
-      <c r="VC12" s="2"/>
-      <c r="VD12" s="2"/>
-      <c r="VE12" s="2"/>
-      <c r="VF12" s="2"/>
-      <c r="VG12" s="2"/>
-      <c r="VH12" s="2"/>
-      <c r="VI12" s="2"/>
-      <c r="VJ12" s="2"/>
-      <c r="VK12" s="2"/>
-      <c r="VL12" s="2"/>
-      <c r="VM12" s="2"/>
-      <c r="VN12" s="2"/>
-      <c r="VO12" s="2"/>
-      <c r="VP12" s="2"/>
-      <c r="VQ12" s="2"/>
-      <c r="VR12" s="2"/>
-      <c r="VS12" s="2"/>
-      <c r="VT12" s="2"/>
-      <c r="VU12" s="2"/>
-      <c r="VV12" s="2"/>
-      <c r="VW12" s="2"/>
-      <c r="VX12" s="2"/>
-      <c r="VY12" s="2"/>
-      <c r="VZ12" s="2"/>
-      <c r="WA12" s="2"/>
-      <c r="WB12" s="2"/>
-      <c r="WC12" s="2"/>
-      <c r="WD12" s="2"/>
-      <c r="WE12" s="2"/>
-      <c r="WF12" s="2"/>
-      <c r="WG12" s="2"/>
-      <c r="WH12" s="2"/>
-      <c r="WI12" s="2"/>
-      <c r="WJ12" s="2"/>
-      <c r="WK12" s="2"/>
-      <c r="WL12" s="2"/>
-      <c r="WM12" s="2"/>
-      <c r="WN12" s="2"/>
-      <c r="WO12" s="2"/>
-      <c r="WP12" s="2"/>
-      <c r="WQ12" s="2"/>
-      <c r="WR12" s="2"/>
-      <c r="WS12" s="2"/>
-      <c r="WT12" s="2"/>
-      <c r="WU12" s="2"/>
-      <c r="WV12" s="2"/>
-      <c r="WW12" s="2"/>
-      <c r="WX12" s="2"/>
-      <c r="WY12" s="2"/>
-      <c r="WZ12" s="2"/>
-      <c r="XA12" s="2"/>
-      <c r="XB12" s="2"/>
-      <c r="XC12" s="2"/>
-      <c r="XD12" s="2"/>
-      <c r="XE12" s="2"/>
-      <c r="XF12" s="2"/>
-      <c r="XG12" s="2"/>
-      <c r="XH12" s="2"/>
-      <c r="XI12" s="2"/>
-      <c r="XJ12" s="2"/>
-      <c r="XK12" s="2"/>
-      <c r="XL12" s="2"/>
-      <c r="XM12" s="2"/>
-      <c r="XN12" s="2"/>
-      <c r="XO12" s="2"/>
-      <c r="XP12" s="2"/>
-      <c r="XQ12" s="2"/>
-      <c r="XR12" s="2"/>
-      <c r="XS12" s="2"/>
-      <c r="XT12" s="2"/>
-      <c r="XU12" s="2"/>
-      <c r="XV12" s="2"/>
-      <c r="XW12" s="2"/>
-      <c r="XX12" s="2"/>
-      <c r="XY12" s="2"/>
-      <c r="XZ12" s="2"/>
-      <c r="YA12" s="2"/>
-      <c r="YB12" s="2"/>
-      <c r="YC12" s="2"/>
-      <c r="YD12" s="2"/>
-      <c r="YE12" s="2"/>
-      <c r="YF12" s="2"/>
-      <c r="YG12" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="2"/>
+      <c r="BG11" s="2"/>
+      <c r="BH11" s="2"/>
+      <c r="BI11" s="2"/>
+      <c r="BJ11" s="2"/>
+      <c r="BK11" s="2"/>
+      <c r="BL11" s="2"/>
+      <c r="BM11" s="2"/>
+      <c r="BN11" s="2"/>
+      <c r="BO11" s="2"/>
+      <c r="BP11" s="2"/>
+      <c r="BQ11" s="2"/>
+      <c r="BR11" s="2"/>
+      <c r="BS11" s="2"/>
+      <c r="BT11" s="2"/>
+      <c r="BU11" s="2"/>
+      <c r="BV11" s="2"/>
+      <c r="BW11" s="2"/>
+      <c r="BX11" s="2"/>
+      <c r="BY11" s="2"/>
+      <c r="BZ11" s="2"/>
+      <c r="CA11" s="2"/>
+      <c r="CB11" s="2"/>
+      <c r="CC11" s="2"/>
+      <c r="CD11" s="2"/>
+      <c r="CE11" s="2"/>
+      <c r="CF11" s="2"/>
+      <c r="CG11" s="2"/>
+      <c r="CH11" s="2"/>
+      <c r="CI11" s="2"/>
+      <c r="CJ11" s="2"/>
+      <c r="CK11" s="2"/>
+      <c r="CL11" s="2"/>
+      <c r="CM11" s="2"/>
+      <c r="CN11" s="2"/>
+      <c r="CO11" s="2"/>
+      <c r="CP11" s="2"/>
+      <c r="CQ11" s="2"/>
+      <c r="CR11" s="2"/>
+      <c r="CS11" s="2"/>
+      <c r="CT11" s="2"/>
+      <c r="CU11" s="2"/>
+      <c r="CV11" s="2"/>
+      <c r="CW11" s="2"/>
+      <c r="CX11" s="2"/>
+      <c r="CY11" s="2"/>
+      <c r="CZ11" s="2"/>
+      <c r="DA11" s="2"/>
+      <c r="DB11" s="2"/>
+      <c r="DC11" s="2"/>
+      <c r="DD11" s="2"/>
+      <c r="DE11" s="2"/>
+      <c r="DF11" s="2"/>
+      <c r="DG11" s="2"/>
+      <c r="DH11" s="2"/>
+      <c r="DI11" s="2"/>
+      <c r="DJ11" s="2"/>
+      <c r="DK11" s="2"/>
+      <c r="DL11" s="2"/>
+      <c r="DM11" s="2"/>
+      <c r="DN11" s="2"/>
+      <c r="DO11" s="2"/>
+      <c r="DP11" s="2"/>
+      <c r="DQ11" s="2"/>
+      <c r="DR11" s="2"/>
+      <c r="DS11" s="2"/>
+      <c r="DT11" s="2"/>
+      <c r="DU11" s="2"/>
+      <c r="DV11" s="2"/>
+      <c r="DW11" s="2"/>
+      <c r="DX11" s="2"/>
+      <c r="DY11" s="2"/>
+      <c r="DZ11" s="2"/>
+      <c r="EA11" s="2"/>
+      <c r="EB11" s="2"/>
+      <c r="EC11" s="2"/>
+      <c r="ED11" s="2"/>
+      <c r="EE11" s="2"/>
+      <c r="EF11" s="2"/>
+      <c r="EG11" s="2"/>
+      <c r="EH11" s="2"/>
+      <c r="EI11" s="2"/>
+      <c r="EJ11" s="2"/>
+      <c r="EK11" s="2"/>
+      <c r="EL11" s="2"/>
+      <c r="EM11" s="2"/>
+      <c r="EN11" s="2"/>
+      <c r="EO11" s="2"/>
+      <c r="EP11" s="2"/>
+      <c r="EQ11" s="2"/>
+      <c r="ER11" s="2"/>
+      <c r="ES11" s="2"/>
+      <c r="ET11" s="2"/>
+      <c r="EU11" s="2"/>
+      <c r="EV11" s="2"/>
+      <c r="EW11" s="2"/>
+      <c r="EX11" s="2"/>
+      <c r="EY11" s="2"/>
+      <c r="EZ11" s="2"/>
+      <c r="FA11" s="2"/>
+      <c r="FB11" s="2"/>
+      <c r="FC11" s="2"/>
+      <c r="FD11" s="2"/>
+      <c r="FE11" s="2"/>
+      <c r="FF11" s="2"/>
+      <c r="FG11" s="2"/>
+      <c r="FH11" s="2"/>
+      <c r="FI11" s="2"/>
+      <c r="FJ11" s="2"/>
+      <c r="FK11" s="2"/>
+      <c r="FL11" s="2"/>
+      <c r="FM11" s="2"/>
+      <c r="FN11" s="2"/>
+      <c r="FO11" s="2"/>
+      <c r="FP11" s="2"/>
+      <c r="FQ11" s="2"/>
+      <c r="FR11" s="2"/>
+      <c r="FS11" s="2"/>
+      <c r="FT11" s="2"/>
+      <c r="FU11" s="2"/>
+      <c r="FV11" s="2"/>
+      <c r="FW11" s="2"/>
+      <c r="FX11" s="2"/>
+      <c r="FY11" s="2"/>
+      <c r="FZ11" s="2"/>
+      <c r="GA11" s="2"/>
+      <c r="GB11" s="2"/>
+      <c r="GC11" s="2"/>
+      <c r="GD11" s="2"/>
+      <c r="GE11" s="2"/>
+      <c r="GF11" s="2"/>
+      <c r="GG11" s="2"/>
+      <c r="GH11" s="2"/>
+      <c r="GI11" s="2"/>
+      <c r="GJ11" s="2"/>
+      <c r="GK11" s="2"/>
+      <c r="GL11" s="2"/>
+      <c r="GM11" s="2"/>
+      <c r="GN11" s="2"/>
+      <c r="GO11" s="2"/>
+      <c r="GP11" s="2"/>
+      <c r="GQ11" s="2"/>
+      <c r="GR11" s="2"/>
+      <c r="GS11" s="2"/>
+      <c r="GT11" s="2"/>
+      <c r="GU11" s="2"/>
+      <c r="GV11" s="2"/>
+      <c r="GW11" s="2"/>
+      <c r="GX11" s="2"/>
+      <c r="GY11" s="2"/>
+      <c r="GZ11" s="2"/>
+      <c r="HA11" s="2"/>
+      <c r="HB11" s="2"/>
+      <c r="HC11" s="2"/>
+      <c r="HD11" s="2"/>
+      <c r="HE11" s="2"/>
+      <c r="HF11" s="2"/>
+      <c r="HG11" s="2"/>
+      <c r="HH11" s="2"/>
+      <c r="HI11" s="2"/>
+      <c r="HJ11" s="2"/>
+      <c r="HK11" s="2"/>
+      <c r="HL11" s="2"/>
+      <c r="HM11" s="2"/>
+      <c r="HN11" s="2"/>
+      <c r="HO11" s="2"/>
+      <c r="HP11" s="2"/>
+      <c r="HQ11" s="2"/>
+      <c r="HR11" s="2"/>
+      <c r="HS11" s="2"/>
+      <c r="HT11" s="2"/>
+      <c r="HU11" s="2"/>
+      <c r="HV11" s="2"/>
+      <c r="HW11" s="2"/>
+      <c r="HX11" s="2"/>
+      <c r="HY11" s="2"/>
+      <c r="HZ11" s="2"/>
+      <c r="IA11" s="2"/>
+      <c r="IB11" s="2"/>
+      <c r="IC11" s="2"/>
+      <c r="ID11" s="2"/>
+      <c r="IE11" s="2"/>
+      <c r="IF11" s="2"/>
+      <c r="IG11" s="2"/>
+      <c r="IH11" s="2"/>
+      <c r="II11" s="2"/>
+      <c r="IJ11" s="2"/>
+      <c r="IK11" s="2"/>
+      <c r="IL11" s="2"/>
+      <c r="IM11" s="2"/>
+      <c r="IN11" s="2"/>
+      <c r="IO11" s="2"/>
+      <c r="IP11" s="2"/>
+      <c r="IQ11" s="2"/>
+      <c r="IR11" s="2"/>
+      <c r="IS11" s="2"/>
+      <c r="IT11" s="2"/>
+      <c r="IU11" s="2"/>
+      <c r="IV11" s="2"/>
+      <c r="IW11" s="2"/>
+      <c r="IX11" s="2"/>
+      <c r="IY11" s="2"/>
+      <c r="IZ11" s="2"/>
+      <c r="JA11" s="2"/>
+      <c r="JB11" s="2"/>
+      <c r="JC11" s="2"/>
+      <c r="JD11" s="2"/>
+      <c r="JE11" s="2"/>
+      <c r="JF11" s="2"/>
+      <c r="JG11" s="2"/>
+      <c r="JH11" s="2"/>
+      <c r="JI11" s="2"/>
+      <c r="JJ11" s="2"/>
+      <c r="JK11" s="2"/>
+      <c r="JL11" s="2"/>
+      <c r="JM11" s="2"/>
+      <c r="JN11" s="2"/>
+      <c r="JO11" s="2"/>
+      <c r="JP11" s="2"/>
+      <c r="JQ11" s="2"/>
+      <c r="JR11" s="2"/>
+      <c r="JS11" s="2"/>
+      <c r="JT11" s="2"/>
+      <c r="JU11" s="2"/>
+      <c r="JV11" s="2"/>
+      <c r="JW11" s="2"/>
+      <c r="JX11" s="2"/>
+      <c r="JY11" s="2"/>
+      <c r="JZ11" s="2"/>
+      <c r="KA11" s="2"/>
+      <c r="KB11" s="2"/>
+      <c r="KC11" s="2"/>
+      <c r="KD11" s="2"/>
+      <c r="KE11" s="2"/>
+      <c r="KF11" s="2"/>
+      <c r="KG11" s="2"/>
+      <c r="KH11" s="2"/>
+      <c r="KI11" s="2"/>
+      <c r="KJ11" s="2"/>
+      <c r="KK11" s="2"/>
+      <c r="KL11" s="2"/>
+      <c r="KM11" s="2"/>
+      <c r="KN11" s="2"/>
+      <c r="KO11" s="2"/>
+      <c r="KP11" s="2"/>
+      <c r="KQ11" s="2"/>
+      <c r="KR11" s="2"/>
+      <c r="KS11" s="2"/>
+      <c r="KT11" s="2"/>
+      <c r="KU11" s="2"/>
+      <c r="KV11" s="2"/>
+      <c r="KW11" s="2"/>
+      <c r="KX11" s="2"/>
+      <c r="KY11" s="2"/>
+      <c r="KZ11" s="2"/>
+      <c r="LA11" s="2"/>
+      <c r="LB11" s="2"/>
+      <c r="LC11" s="2"/>
+      <c r="LD11" s="2"/>
+      <c r="LE11" s="2"/>
+      <c r="LF11" s="2"/>
+      <c r="LG11" s="2"/>
+      <c r="LH11" s="2"/>
+      <c r="LI11" s="2"/>
+      <c r="LJ11" s="2"/>
+      <c r="LK11" s="2"/>
+      <c r="LL11" s="2"/>
+      <c r="LM11" s="2"/>
+      <c r="LN11" s="2"/>
+      <c r="LO11" s="2"/>
+      <c r="LP11" s="2"/>
+      <c r="LQ11" s="2"/>
+      <c r="LR11" s="2"/>
+      <c r="LS11" s="2"/>
+      <c r="LT11" s="2"/>
+      <c r="LU11" s="2"/>
+      <c r="LV11" s="2"/>
+      <c r="LW11" s="2"/>
+      <c r="LX11" s="2"/>
+      <c r="LY11" s="2"/>
+      <c r="LZ11" s="2"/>
+      <c r="MA11" s="2"/>
+      <c r="MB11" s="2"/>
+      <c r="MC11" s="2"/>
+      <c r="MD11" s="2"/>
+      <c r="ME11" s="2"/>
+      <c r="MF11" s="2"/>
+      <c r="MG11" s="2"/>
+      <c r="MH11" s="2"/>
+      <c r="MI11" s="2"/>
+      <c r="MJ11" s="2"/>
+      <c r="MK11" s="2"/>
+      <c r="ML11" s="2"/>
+      <c r="MM11" s="2"/>
+      <c r="MN11" s="2"/>
+      <c r="MO11" s="2"/>
+      <c r="MP11" s="2"/>
+      <c r="MQ11" s="2"/>
+      <c r="MR11" s="2"/>
+      <c r="MS11" s="2"/>
+      <c r="MT11" s="2"/>
+      <c r="MU11" s="2"/>
+      <c r="MV11" s="2"/>
+      <c r="MW11" s="2"/>
+      <c r="MX11" s="2"/>
+      <c r="MY11" s="2"/>
+      <c r="MZ11" s="2"/>
+      <c r="NA11" s="2"/>
+      <c r="NB11" s="2"/>
+      <c r="NC11" s="2"/>
+      <c r="ND11" s="2"/>
+      <c r="NE11" s="2"/>
+      <c r="NF11" s="2"/>
+      <c r="NG11" s="2"/>
+      <c r="NH11" s="2"/>
+      <c r="NI11" s="2"/>
+      <c r="NJ11" s="2"/>
+      <c r="NK11" s="2"/>
+      <c r="NL11" s="2"/>
+      <c r="NM11" s="2"/>
+      <c r="NN11" s="2"/>
+      <c r="NO11" s="2"/>
+      <c r="NP11" s="2"/>
+      <c r="NQ11" s="2"/>
+      <c r="NR11" s="2"/>
+      <c r="NS11" s="2"/>
+      <c r="NT11" s="2"/>
+      <c r="NU11" s="2"/>
+      <c r="NV11" s="2"/>
+      <c r="NW11" s="2"/>
+      <c r="NX11" s="2"/>
+      <c r="NY11" s="2"/>
+      <c r="NZ11" s="2"/>
+      <c r="OA11" s="2"/>
+      <c r="OB11" s="2"/>
+      <c r="OC11" s="2"/>
+      <c r="OD11" s="2"/>
+      <c r="OE11" s="2"/>
+      <c r="OF11" s="2"/>
+      <c r="OG11" s="2"/>
+      <c r="OH11" s="2"/>
+      <c r="OI11" s="2"/>
+      <c r="OJ11" s="2"/>
+      <c r="OK11" s="2"/>
+      <c r="OL11" s="2"/>
+      <c r="OM11" s="2"/>
+      <c r="ON11" s="2"/>
+      <c r="OO11" s="2"/>
+      <c r="OP11" s="2"/>
+      <c r="OQ11" s="2"/>
+      <c r="OR11" s="2"/>
+      <c r="OS11" s="2"/>
+      <c r="OT11" s="2"/>
+      <c r="OU11" s="2"/>
+      <c r="OV11" s="2"/>
+      <c r="OW11" s="2"/>
+      <c r="OX11" s="2"/>
+      <c r="OY11" s="2"/>
+      <c r="OZ11" s="2"/>
+      <c r="PA11" s="2"/>
+      <c r="PB11" s="2"/>
+      <c r="PC11" s="2"/>
+      <c r="PD11" s="2"/>
+      <c r="PE11" s="2"/>
+      <c r="PF11" s="2"/>
+      <c r="PG11" s="2"/>
+      <c r="PH11" s="2"/>
+      <c r="PI11" s="2"/>
+      <c r="PJ11" s="2"/>
+      <c r="PK11" s="2"/>
+      <c r="PL11" s="2"/>
+      <c r="PM11" s="2"/>
+      <c r="PN11" s="2"/>
+      <c r="PO11" s="2"/>
+      <c r="PP11" s="2"/>
+      <c r="PQ11" s="2"/>
+      <c r="PR11" s="2"/>
+      <c r="PS11" s="2"/>
+      <c r="PT11" s="2"/>
+      <c r="PU11" s="2"/>
+      <c r="PV11" s="2"/>
+      <c r="PW11" s="2"/>
+      <c r="PX11" s="2"/>
+      <c r="PY11" s="2"/>
+      <c r="PZ11" s="2"/>
+      <c r="QA11" s="2"/>
+      <c r="QB11" s="2"/>
+      <c r="QC11" s="2"/>
+      <c r="QD11" s="2"/>
+      <c r="QE11" s="2"/>
+      <c r="QF11" s="2"/>
+      <c r="QG11" s="2"/>
+      <c r="QH11" s="2"/>
+      <c r="QI11" s="2"/>
+      <c r="QJ11" s="2"/>
+      <c r="QK11" s="2"/>
+      <c r="QL11" s="2"/>
+      <c r="QM11" s="2"/>
+      <c r="QN11" s="2"/>
+      <c r="QO11" s="2"/>
+      <c r="QP11" s="2"/>
+      <c r="QQ11" s="2"/>
+      <c r="QR11" s="2"/>
+      <c r="QS11" s="2"/>
+      <c r="QT11" s="2"/>
+      <c r="QU11" s="2"/>
+      <c r="QV11" s="2"/>
+      <c r="QW11" s="2"/>
+      <c r="QX11" s="2"/>
+      <c r="QY11" s="2"/>
+      <c r="QZ11" s="2"/>
+      <c r="RA11" s="2"/>
+      <c r="RB11" s="2"/>
+      <c r="RC11" s="2"/>
+      <c r="RD11" s="2"/>
+      <c r="RE11" s="2"/>
+      <c r="RF11" s="2"/>
+      <c r="RG11" s="2"/>
+      <c r="RH11" s="2"/>
+      <c r="RI11" s="2"/>
+      <c r="RJ11" s="2"/>
+      <c r="RK11" s="2"/>
+      <c r="RL11" s="2"/>
+      <c r="RM11" s="2"/>
+      <c r="RN11" s="2"/>
+      <c r="RO11" s="2"/>
+      <c r="RP11" s="2"/>
+      <c r="RQ11" s="2"/>
+      <c r="RR11" s="2"/>
+      <c r="RS11" s="2"/>
+      <c r="RT11" s="2"/>
+      <c r="RU11" s="2"/>
+      <c r="RV11" s="2"/>
+      <c r="RW11" s="2"/>
+      <c r="RX11" s="2"/>
+      <c r="RY11" s="2"/>
+      <c r="RZ11" s="2"/>
+      <c r="SA11" s="2"/>
+      <c r="SB11" s="2"/>
+      <c r="SC11" s="2"/>
+      <c r="SD11" s="2"/>
+      <c r="SE11" s="2"/>
+      <c r="SF11" s="2"/>
+      <c r="SG11" s="2"/>
+      <c r="SH11" s="2"/>
+      <c r="SI11" s="2"/>
+      <c r="SJ11" s="2"/>
+      <c r="SK11" s="2"/>
+      <c r="SL11" s="2"/>
+      <c r="SM11" s="2"/>
+      <c r="SN11" s="2"/>
+      <c r="SO11" s="2"/>
+      <c r="SP11" s="2"/>
+      <c r="SQ11" s="2"/>
+      <c r="SR11" s="2"/>
+      <c r="SS11" s="2"/>
+      <c r="ST11" s="2"/>
+      <c r="SU11" s="2"/>
+      <c r="SV11" s="2"/>
+      <c r="SW11" s="2"/>
+      <c r="SX11" s="2"/>
+      <c r="SY11" s="2"/>
+      <c r="SZ11" s="2"/>
+      <c r="TA11" s="2"/>
+      <c r="TB11" s="2"/>
+      <c r="TC11" s="2"/>
+      <c r="TD11" s="2"/>
+      <c r="TE11" s="2"/>
+      <c r="TF11" s="2"/>
+      <c r="TG11" s="2"/>
+      <c r="TH11" s="2"/>
+      <c r="TI11" s="2"/>
+      <c r="TJ11" s="2"/>
+      <c r="TK11" s="2"/>
+      <c r="TL11" s="2"/>
+      <c r="TM11" s="2"/>
+      <c r="TN11" s="2"/>
+      <c r="TO11" s="2"/>
+      <c r="TP11" s="2"/>
+      <c r="TQ11" s="2"/>
+      <c r="TR11" s="2"/>
+      <c r="TS11" s="2"/>
+      <c r="TT11" s="2"/>
+      <c r="TU11" s="2"/>
+      <c r="TV11" s="2"/>
+      <c r="TW11" s="2"/>
+      <c r="TX11" s="2"/>
+      <c r="TY11" s="2"/>
+      <c r="TZ11" s="2"/>
+      <c r="UA11" s="2"/>
+      <c r="UB11" s="2"/>
+      <c r="UC11" s="2"/>
+      <c r="UD11" s="2"/>
+      <c r="UE11" s="2"/>
+      <c r="UF11" s="2"/>
+      <c r="UG11" s="2"/>
+      <c r="UH11" s="2"/>
+      <c r="UI11" s="2"/>
+      <c r="UJ11" s="2"/>
+      <c r="UK11" s="2"/>
+      <c r="UL11" s="2"/>
+      <c r="UM11" s="2"/>
+      <c r="UN11" s="2"/>
+      <c r="UO11" s="2"/>
+      <c r="UP11" s="2"/>
+      <c r="UQ11" s="2"/>
+      <c r="UR11" s="2"/>
+      <c r="US11" s="2"/>
+      <c r="UT11" s="2"/>
+      <c r="UU11" s="2"/>
+      <c r="UV11" s="2"/>
+      <c r="UW11" s="2"/>
+      <c r="UX11" s="2"/>
+      <c r="UY11" s="2"/>
+      <c r="UZ11" s="2"/>
+      <c r="VA11" s="2"/>
+      <c r="VB11" s="2"/>
+      <c r="VC11" s="2"/>
+      <c r="VD11" s="2"/>
+      <c r="VE11" s="2"/>
+      <c r="VF11" s="2"/>
+      <c r="VG11" s="2"/>
+      <c r="VH11" s="2"/>
+      <c r="VI11" s="2"/>
+      <c r="VJ11" s="2"/>
+      <c r="VK11" s="2"/>
+      <c r="VL11" s="2"/>
+      <c r="VM11" s="2"/>
+      <c r="VN11" s="2"/>
+      <c r="VO11" s="2"/>
+      <c r="VP11" s="2"/>
+      <c r="VQ11" s="2"/>
+      <c r="VR11" s="2"/>
+      <c r="VS11" s="2"/>
+      <c r="VT11" s="2"/>
+      <c r="VU11" s="2"/>
+      <c r="VV11" s="2"/>
+      <c r="VW11" s="2"/>
+      <c r="VX11" s="2"/>
+      <c r="VY11" s="2"/>
+      <c r="VZ11" s="2"/>
+      <c r="WA11" s="2"/>
+      <c r="WB11" s="2"/>
+      <c r="WC11" s="2"/>
+      <c r="WD11" s="2"/>
+      <c r="WE11" s="2"/>
+      <c r="WF11" s="2"/>
+      <c r="WG11" s="2"/>
+      <c r="WH11" s="2"/>
+      <c r="WI11" s="2"/>
+      <c r="WJ11" s="2"/>
+      <c r="WK11" s="2"/>
+      <c r="WL11" s="2"/>
+      <c r="WM11" s="2"/>
+      <c r="WN11" s="2"/>
+      <c r="WO11" s="2"/>
+      <c r="WP11" s="2"/>
+      <c r="WQ11" s="2"/>
+      <c r="WR11" s="2"/>
+      <c r="WS11" s="2"/>
+      <c r="WT11" s="2"/>
+      <c r="WU11" s="2"/>
+      <c r="WV11" s="2"/>
+      <c r="WW11" s="2"/>
+      <c r="WX11" s="2"/>
+      <c r="WY11" s="2"/>
+      <c r="WZ11" s="2"/>
+      <c r="XA11" s="2"/>
+      <c r="XB11" s="2"/>
+      <c r="XC11" s="2"/>
+      <c r="XD11" s="2"/>
+      <c r="XE11" s="2"/>
+      <c r="XF11" s="2"/>
+      <c r="XG11" s="2"/>
+      <c r="XH11" s="2"/>
+      <c r="XI11" s="2"/>
+      <c r="XJ11" s="2"/>
+      <c r="XK11" s="2"/>
+      <c r="XL11" s="2"/>
+      <c r="XM11" s="2"/>
+      <c r="XN11" s="2"/>
+      <c r="XO11" s="2"/>
+      <c r="XP11" s="2"/>
+      <c r="XQ11" s="2"/>
+      <c r="XR11" s="2"/>
+      <c r="XS11" s="2"/>
+      <c r="XT11" s="2"/>
+      <c r="XU11" s="2"/>
+      <c r="XV11" s="2"/>
+      <c r="XW11" s="2"/>
+      <c r="XX11" s="2"/>
+      <c r="XY11" s="2"/>
+      <c r="XZ11" s="2"/>
+      <c r="YA11" s="2"/>
+      <c r="YB11" s="2"/>
+      <c r="YC11" s="2"/>
+      <c r="YD11" s="2"/>
+      <c r="YE11" s="2"/>
+      <c r="YF11" s="2"/>
+      <c r="YG11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>